<commit_message>
Lit review started for intro
</commit_message>
<xml_diff>
--- a/Write up/lit_review_methods.xlsx
+++ b/Write up/lit_review_methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228AE28C-8A7C-4D6F-B68E-5DE36BF9E9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAA2950-A50D-48AD-A531-152A16D21621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F275550-1BB5-47D6-B7A4-69193C16D8D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Authors</t>
   </si>
@@ -104,7 +104,28 @@
     <t>Mixed models. Use data from 63 countries. Use range of governance, econoimc, social variables. Models are at the country scale</t>
   </si>
   <si>
-    <t xml:space="preserve">Doing this at the country scale might mean less variation? </t>
+    <t>Doing this at the country scale might mean less variation? Also much longer time series. Also, no diagnostics apart from R2, and no statement of variation for fixed or random effects</t>
+  </si>
+  <si>
+    <t>Bonilla-Bedoya et al</t>
+  </si>
+  <si>
+    <t>Socioecological system and potential deforestatino in Western Amazon forest landscapes</t>
+  </si>
+  <si>
+    <t>Modelling potential land use change. Detemined whether there were relationships between vulnerability to forest loss and the management policies</t>
+  </si>
+  <si>
+    <t>Uses biophysical and socioeconomic variables. Use maximum entropy model.</t>
+  </si>
+  <si>
+    <t>I think quite nice, although I need to read up a bit on entropy models. They cite Souza and De Marco 2014 who go into it.</t>
+  </si>
+  <si>
+    <t>Souza &amp; De Marco</t>
+  </si>
+  <si>
+    <t>The use of species distribution models to predict the spatial distribution of deforestation in the western Brazilian Amazon</t>
   </si>
 </sst>
 </file>
@@ -468,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA9A1CB-69B7-4A9F-B5E8-04F259C3C63C}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,14 +584,48 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>2018</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>2014</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2014</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated lit review excel
</commit_message>
<xml_diff>
--- a/Write up/lit_review_methods.xlsx
+++ b/Write up/lit_review_methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB08FCD-A18C-4CA2-99D9-39FFF30F3450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C143A9-6E64-48BE-9B13-E3A20FC72A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F275550-1BB5-47D6-B7A4-69193C16D8D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Authors</t>
   </si>
@@ -210,13 +210,103 @@
   </si>
   <si>
     <t xml:space="preserve">Country-scale. Also don't report any variance </t>
+  </si>
+  <si>
+    <t>Curtis et al</t>
+  </si>
+  <si>
+    <t>Classifying drivers of global forest loss</t>
+  </si>
+  <si>
+    <t>Developed a forest loss classification model that identified dominant drivers of land cover and land use change between 2001 and 2015. 27% of global forest loss resulted from permenent land use change for commodity production</t>
+  </si>
+  <si>
+    <t>Good citation for global driver of forest loss being commodity production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egli et al </t>
+  </si>
+  <si>
+    <t>Winners and losers of national and global efforts to reconcile agricultural intensification and biodiversity conservation</t>
+  </si>
+  <si>
+    <t>Used spatial optimisation to identify yield gaps and areas of high biodiversity, so as to identify where in the world you could intensify agriculture and cause the least damage to biodiversity</t>
+  </si>
+  <si>
+    <t>Nice idea, and a good argument for global cooperation in food planning and production. But key point is that there would be winners and losers in terms of economic development, food security, food sovereignty, and conservation. You could still implement national optimisation and achieve conservation beenfits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estoque et al </t>
+  </si>
+  <si>
+    <t>The future of Southeast Asia's forests</t>
+  </si>
+  <si>
+    <t>employ land change model to investigate 5 shared socioeconomic pathways to portray plausible future scenarios. Worst case scenario SEA forest would lose 5.2M ha. Best case scenario the would gain 19.6M ha.</t>
+  </si>
+  <si>
+    <t>Quite complicated methods. They use the Shared Socioeconomic Pathways (SSP) scenarios, which are pre-existing and are develped for climate change research. For the transition potential modelling, they used only biophysical variables (including things like distance to roads)</t>
+  </si>
+  <si>
+    <t>Spatial analysis, using land use change maps and biophysical and human physical characteristics. Integrated with the SSP pathways. As with some of the above spatial analyses - they require variables to be spatially explicit and at the correct scale (ie cell size). So not the way to identify trends at, say, national level</t>
+  </si>
+  <si>
+    <t>Ewers</t>
+  </si>
+  <si>
+    <t>Interaction e ffects between economic development and forest cover determine deforestation rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple regression and ANOVAs. Doesn't use mixed models. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He adds interaction effects and found that high-income nations show the opposite response to disappearing forest cover than ow-income nations. High-incomce countries with low forest cover have the highest rates of afforestation. Low-income countries with little forest are more likely to lose that faster proportionally than low-income countires with high forest cover. Nations with large amounts of forest have equal defor rates, regardless of national wealth.</t>
+  </si>
+  <si>
+    <t>Does this suffer from pseudoreplication? He's not accounting for the fact that there are repeat measurements. Might give overly small Ses and incorrect effect sizes?</t>
+  </si>
+  <si>
+    <t>Gao &amp; Liu</t>
+  </si>
+  <si>
+    <t>Deforestation in Heilongjiang Province of China, 1896-2000: Severity, spatiotemporal patterns and causes</t>
+  </si>
+  <si>
+    <t>Used forest cover maps from different periods to assess land use change. IN the past deforestation was large areas, whereas in more recnt times the defor areas are thousands of smaller patches that are getting smaller. They posit that the causes are demand for timber, population-driven land reclamation, and urbanisation.</t>
+  </si>
+  <si>
+    <t>Land use maps from different periods. Overlaid with biophysical variables. They then simply say the "do some statistics". Very poorly described methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very poorly described methods, so it is not clear how they determined relationships between changes in land use and the variables. They arrive at their conclusions about drivers by hypothesising. </t>
+  </si>
+  <si>
+    <t>Gong et al</t>
+  </si>
+  <si>
+    <t>Determining socioeconoimc drivers of urban forest fragmentation with historical remote sensing images</t>
+  </si>
+  <si>
+    <t>Logistic regression models used to predict socioeconoimc variables (not really sure what is going on there)? Then step-wise multiple regression to examine causal relationships between forest fragmentation and socioeconoimcs</t>
+  </si>
+  <si>
+    <t>Used multiple regression to identify socioeconoimc drives of urban fores fragmentation in a mega city in China.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very fine scale - single location. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Considers cellualr automata to be appropriate way of modelling land use change from the bottom up. Claim that it is at the local level that complex processes that underlie fundamental changes observed in the land use system can be captured </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very cool. But again, very spatial in nature. Its all about cells and the proximity of cells to one another </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,7 +316,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -253,10 +350,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -573,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA9A1CB-69B7-4A9F-B5E8-04F259C3C63C}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,215 +706,346 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>2016</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2004</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2004</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>2018</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2014</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>2013</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>2019</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>2015</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>2008</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>2007</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="12" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="191.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B19" s="2">
         <v>2014</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to lit review excel
</commit_message>
<xml_diff>
--- a/Write up/lit_review_methods.xlsx
+++ b/Write up/lit_review_methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A58F1C-9A4E-4CC0-93B3-96718788D1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32AE61D-87FE-447F-AFC8-46DF56C0DDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F275550-1BB5-47D6-B7A4-69193C16D8D2}"/>
   </bookViews>
@@ -673,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA9A1CB-69B7-4A9F-B5E8-04F259C3C63C}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>